<commit_message>
Se copia el fichero del tiempo a la carpeta de entrenamiento
Es necesario por el momento que los ficheros esten en la misma carpeta para que se puedan importar las funciones. En la carpeta Weather se mantiene una copia del original
</commit_message>
<xml_diff>
--- a/Entrenamientos/Procesado_Tramos.xlsx
+++ b/Entrenamientos/Procesado_Tramos.xlsx
@@ -480,7 +480,7 @@
         <v>32.80754716981132</v>
       </c>
       <c r="I2">
-        <v>8.398054349425172</v>
+        <v>6.718880072643945</v>
       </c>
       <c r="J2">
         <v>-3.377386253851977</v>
@@ -515,7 +515,7 @@
         <v>17.70244897959184</v>
       </c>
       <c r="I3">
-        <v>5.337415225736499</v>
+        <v>7.188764034610809</v>
       </c>
       <c r="J3">
         <v>4.181099517057391</v>
@@ -550,7 +550,7 @@
         <v>38.7765673907564</v>
       </c>
       <c r="I4">
-        <v>8.311220482970354</v>
+        <v>8.537488609571749</v>
       </c>
       <c r="J4">
         <v>-1.737872666585584</v>
@@ -585,7 +585,7 @@
         <v>24.39670806006297</v>
       </c>
       <c r="I5">
-        <v>8.704790950921202</v>
+        <v>8.334436920592802</v>
       </c>
       <c r="J5">
         <v>2.662584888997575</v>
@@ -620,7 +620,7 @@
         <v>35.43781081186982</v>
       </c>
       <c r="I6">
-        <v>8.487545683986143</v>
+        <v>8.287183163245322</v>
       </c>
       <c r="J6">
         <v>-0.8731442972049492</v>
@@ -655,7 +655,7 @@
         <v>26.91783553264644</v>
       </c>
       <c r="I7">
-        <v>8.945233376482218</v>
+        <v>8.076852881656638</v>
       </c>
       <c r="J7">
         <v>1.566720145088133</v>
@@ -690,7 +690,7 @@
         <v>36.10140845070423</v>
       </c>
       <c r="I8">
-        <v>8.230975671044503</v>
+        <v>8.56213797538183</v>
       </c>
       <c r="J8">
         <v>-1.730661365554174</v>
@@ -725,7 +725,7 @@
         <v>22.79205298013245</v>
       </c>
       <c r="I9">
-        <v>4.616644365128644</v>
+        <v>7.106877752374618</v>
       </c>
       <c r="J9">
         <v>2.126106682856453</v>
@@ -760,7 +760,7 @@
         <v>32.62</v>
       </c>
       <c r="I10">
-        <v>3.116946362487347</v>
+        <v>7.323880951596324</v>
       </c>
       <c r="J10">
         <v>-1.471856597029948</v>
@@ -795,7 +795,7 @@
         <v>27.13846153846154</v>
       </c>
       <c r="I11">
-        <v>-0.3908086359155407</v>
+        <v>5.706683039617634</v>
       </c>
       <c r="J11">
         <v>0.9465169220567421</v>
@@ -830,7 +830,7 @@
         <v>29.6390977443609</v>
       </c>
       <c r="I12">
-        <v>-1.977512881772691</v>
+        <v>3.616604361784696</v>
       </c>
       <c r="J12">
         <v>-2.440001133357963</v>
@@ -865,7 +865,7 @@
         <v>21.25945945945946</v>
       </c>
       <c r="I13">
-        <v>7.950308951210347</v>
+        <v>6.385003386747204</v>
       </c>
       <c r="J13">
         <v>1.298544674678431</v>
@@ -900,7 +900,7 @@
         <v>21.6</v>
       </c>
       <c r="I14">
-        <v>-3.506416232209443</v>
+        <v>3.28757060155861</v>
       </c>
       <c r="J14">
         <v>-0.09846400393674533</v>
@@ -935,7 +935,7 @@
         <v>19.8</v>
       </c>
       <c r="I15">
-        <v>-4.267735505371278</v>
+        <v>3.829411994305022</v>
       </c>
       <c r="J15">
         <v>0.02355105669742195</v>
@@ -970,7 +970,7 @@
         <v>21.68780487804878</v>
       </c>
       <c r="I16">
-        <v>-6.259535033174609</v>
+        <v>0.5569962249646718</v>
       </c>
       <c r="J16">
         <v>-0.3152407746079614</v>
@@ -1005,7 +1005,7 @@
         <v>18.07714285714286</v>
       </c>
       <c r="I17">
-        <v>-7.570676244388451</v>
+        <v>-0.7650534190750016</v>
       </c>
       <c r="J17">
         <v>2.748246277907367</v>
@@ -1040,7 +1040,7 @@
         <v>31.77931034482759</v>
       </c>
       <c r="I18">
-        <v>5.259195490189875</v>
+        <v>8.441622681669067</v>
       </c>
       <c r="J18">
         <v>-1.301929894925088</v>
@@ -1075,7 +1075,7 @@
         <v>26.67692307692308</v>
       </c>
       <c r="I19">
-        <v>3.102606466876431</v>
+        <v>7.539225509225335</v>
       </c>
       <c r="J19">
         <v>0.9412607962124625</v>
@@ -1110,7 +1110,7 @@
         <v>33.02068965517242</v>
       </c>
       <c r="I20">
-        <v>4.57911472400138</v>
+        <v>8.494772502083276</v>
       </c>
       <c r="J20">
         <v>-0.1707701913945889</v>
@@ -1145,7 +1145,7 @@
         <v>20.44969097651422</v>
       </c>
       <c r="I21">
-        <v>1.457547453191681</v>
+        <v>5.941844580591718</v>
       </c>
       <c r="J21">
         <v>3.207282538011377</v>
@@ -1180,7 +1180,7 @@
         <v>31.37142857142857</v>
       </c>
       <c r="I22">
-        <v>9.846610292454871</v>
+        <v>7.236038465282856</v>
       </c>
       <c r="J22">
         <v>-0.4514696722955265</v>
@@ -1215,7 +1215,7 @@
         <v>12.13256066642521</v>
       </c>
       <c r="I23">
-        <v>-2.454714300246378</v>
+        <v>2.502076994879012</v>
       </c>
       <c r="J23">
         <v>7.137194690917319</v>
@@ -1250,7 +1250,7 @@
         <v>47.53605674776351</v>
       </c>
       <c r="I24">
-        <v>4.404729852307504</v>
+        <v>-0.002796167776577398</v>
       </c>
       <c r="J24">
         <v>-6.677409634473724</v>
@@ -1285,7 +1285,7 @@
         <v>17.60590115492487</v>
       </c>
       <c r="I25">
-        <v>7.887427645537111</v>
+        <v>5.810498478683816</v>
       </c>
       <c r="J25">
         <v>4.067062353848582</v>
@@ -1320,7 +1320,7 @@
         <v>28.13966444743631</v>
       </c>
       <c r="I26">
-        <v>5.056344866232041</v>
+        <v>5.807017494512465</v>
       </c>
       <c r="J26">
         <v>-1.276232235789343</v>
@@ -1355,7 +1355,7 @@
         <v>20.54769526153866</v>
       </c>
       <c r="I27">
-        <v>9.278316107395254</v>
+        <v>3.601939437338369</v>
       </c>
       <c r="J27">
         <v>1.081617389707073</v>
@@ -1390,7 +1390,7 @@
         <v>25.38010633896338</v>
       </c>
       <c r="I28">
-        <v>10.00727702910884</v>
+        <v>2.334200061116734</v>
       </c>
       <c r="J28">
         <v>-0.05371798932544905</v>
@@ -1425,7 +1425,7 @@
         <v>29.42998006103444</v>
       </c>
       <c r="I29">
-        <v>5.775413080352321</v>
+        <v>1.086342238448854</v>
       </c>
       <c r="J29">
         <v>0.01885092567751133</v>
@@ -1460,7 +1460,7 @@
         <v>20.32726804703416</v>
       </c>
       <c r="I30">
-        <v>18.93986484663641</v>
+        <v>1.39947728708304</v>
       </c>
       <c r="J30">
         <v>-0.06144829650640202</v>
@@ -1495,7 +1495,7 @@
         <v>28.0071253153219</v>
       </c>
       <c r="I31">
-        <v>6.786423062899546</v>
+        <v>0.5584160930568689</v>
       </c>
       <c r="J31">
         <v>0.07266559092139174</v>
@@ -1530,7 +1530,7 @@
         <v>27.95151192780667</v>
       </c>
       <c r="I32">
-        <v>7.871285778640685</v>
+        <v>5.89401496715644</v>
       </c>
       <c r="J32">
         <v>-0.9331496626999246</v>
@@ -1565,7 +1565,7 @@
         <v>11.20063333591093</v>
       </c>
       <c r="I33">
-        <v>0.7993149398668953</v>
+        <v>5.547823221084662</v>
       </c>
       <c r="J33">
         <v>5.87039853876158</v>
@@ -1600,7 +1600,7 @@
         <v>45.06607272037013</v>
       </c>
       <c r="I34">
-        <v>-0.8884574423001855</v>
+        <v>-5.62168658079019</v>
       </c>
       <c r="J34">
         <v>-5.723635454283758</v>
@@ -1635,7 +1635,7 @@
         <v>22.31700710400023</v>
       </c>
       <c r="I35">
-        <v>6.266983630717996</v>
+        <v>-0.5916736223585768</v>
       </c>
       <c r="J35">
         <v>2.2907587864157</v>
@@ -1670,7 +1670,7 @@
         <v>44.31840700515254</v>
       </c>
       <c r="I36">
-        <v>5.733329626165953</v>
+        <v>-1.527322503809172</v>
       </c>
       <c r="J36">
         <v>-2.914999449869391</v>
@@ -1705,7 +1705,7 @@
         <v>11.53735976391224</v>
       </c>
       <c r="I37">
-        <v>5.901785938422873</v>
+        <v>5.382536596527786</v>
       </c>
       <c r="J37">
         <v>6.468742984298455</v>
@@ -1740,7 +1740,7 @@
         <v>35.09397199698113</v>
       </c>
       <c r="I38">
-        <v>-6.061655746558085</v>
+        <v>-5.888097786535972</v>
       </c>
       <c r="J38">
         <v>-6.498721130377167</v>
@@ -1775,7 +1775,7 @@
         <v>16.36564704052924</v>
       </c>
       <c r="I39">
-        <v>-9.661135274085868</v>
+        <v>-8.368337017659927</v>
       </c>
       <c r="J39">
         <v>0.3175271552633955</v>
@@ -1810,7 +1810,7 @@
         <v>3.481315565160808</v>
       </c>
       <c r="I40">
-        <v>-3.359145873822522</v>
+        <v>-2.877962773870295</v>
       </c>
       <c r="J40">
         <v>-0.03074911665607301</v>
@@ -1880,7 +1880,7 @@
         <v>32.73</v>
       </c>
       <c r="I42">
-        <v>-9.183888453986818</v>
+        <v>-7.835964729591293</v>
       </c>
       <c r="J42">
         <v>-1.657457684400672</v>
@@ -1915,7 +1915,7 @@
         <v>24.45912550312148</v>
       </c>
       <c r="I43">
-        <v>-9.736325498022939</v>
+        <v>-7.931273967861245</v>
       </c>
       <c r="J43">
         <v>1.799504338098796</v>
@@ -1950,7 +1950,7 @@
         <v>28.14542659877371</v>
       </c>
       <c r="I44">
-        <v>-9.859221056492002</v>
+        <v>-7.087619983992449</v>
       </c>
       <c r="J44">
         <v>-0.5937167895368255</v>
@@ -1985,7 +1985,7 @@
         <v>20.63337665976075</v>
       </c>
       <c r="I45">
-        <v>-9.465449710227134</v>
+        <v>-7.465045819727705</v>
       </c>
       <c r="J45">
         <v>0.5476768680251723</v>
@@ -2020,7 +2020,7 @@
         <v>32.96142121817398</v>
       </c>
       <c r="I46">
-        <v>-9.296934619476286</v>
+        <v>-7.783313432754607</v>
       </c>
       <c r="J46">
         <v>-2.485577973149411</v>
@@ -2055,7 +2055,7 @@
         <v>22.80529998071035</v>
       </c>
       <c r="I47">
-        <v>-7.710675015020469</v>
+        <v>-8.403215743539377</v>
       </c>
       <c r="J47">
         <v>0.6105103008700864</v>
@@ -2090,7 +2090,7 @@
         <v>26.44996819847742</v>
       </c>
       <c r="I48">
-        <v>-7.359421157797521</v>
+        <v>-8.369434130746191</v>
       </c>
       <c r="J48">
         <v>-0.8141979409781851</v>
@@ -2125,7 +2125,7 @@
         <v>23.51841125057711</v>
       </c>
       <c r="I49">
-        <v>-4.762835715620752</v>
+        <v>-8.327633901514552</v>
       </c>
       <c r="J49">
         <v>0.6893167447346721</v>
@@ -2160,7 +2160,7 @@
         <v>29.66697429773181</v>
       </c>
       <c r="I50">
-        <v>-2.826883495187809</v>
+        <v>-7.725948234674917</v>
       </c>
       <c r="J50">
         <v>-1.34259896152115</v>
@@ -2195,7 +2195,7 @@
         <v>24.75771044571406</v>
       </c>
       <c r="I51">
-        <v>-5.64236320507177</v>
+        <v>-7.868465827757365</v>
       </c>
       <c r="J51">
         <v>1.178195346753106</v>
@@ -2230,7 +2230,7 @@
         <v>0.7700523015613591</v>
       </c>
       <c r="I52">
-        <v>-5.120532246198452</v>
+        <v>-9.098386682999061</v>
       </c>
       <c r="J52">
         <v>-0.3038176433854838</v>
@@ -2265,7 +2265,7 @@
         <v>21.35855738879973</v>
       </c>
       <c r="I53">
-        <v>-4.543822948221775</v>
+        <v>-8.488697919854321</v>
       </c>
       <c r="J53">
         <v>1.358546208253752</v>
@@ -2300,7 +2300,7 @@
         <v>32.6115527622473</v>
       </c>
       <c r="I54">
-        <v>-3.52683770209774</v>
+        <v>-8.118368101500197</v>
       </c>
       <c r="J54">
         <v>-1.139542824991412</v>
@@ -2335,7 +2335,7 @@
         <v>29.88282461923664</v>
       </c>
       <c r="I55">
-        <v>-4.710857513066893</v>
+        <v>-10.04810713943173</v>
       </c>
       <c r="J55">
         <v>0.04537913777165534</v>
@@ -2370,7 +2370,7 @@
         <v>32.78954931638728</v>
       </c>
       <c r="I56">
-        <v>-3.514583005744094</v>
+        <v>-8.052791183651516</v>
       </c>
       <c r="J56">
         <v>-0.1902297130857436</v>
@@ -2405,7 +2405,7 @@
         <v>34.37987948243972</v>
       </c>
       <c r="I57">
-        <v>-2.622278686927893</v>
+        <v>-7.185857487220533</v>
       </c>
       <c r="J57">
         <v>0.1149593061108437</v>
@@ -2440,7 +2440,7 @@
         <v>31.37409791999962</v>
       </c>
       <c r="I58">
-        <v>-2.994639762034303</v>
+        <v>-7.267155401158425</v>
       </c>
       <c r="J58">
         <v>-0.05843205651050678</v>
@@ -2475,7 +2475,7 @@
         <v>18.87776233271579</v>
       </c>
       <c r="I59">
-        <v>-4.127355202262784</v>
+        <v>-9.452838846704868</v>
       </c>
       <c r="J59">
         <v>0.1280138098027941</v>
@@ -2510,7 +2510,7 @@
         <v>36.53175163939478</v>
       </c>
       <c r="I60">
-        <v>-3.710701519198039</v>
+        <v>-8.178317322483403</v>
       </c>
       <c r="J60">
         <v>-0.06251000782110948</v>
@@ -2545,7 +2545,7 @@
         <v>29.71279859263217</v>
       </c>
       <c r="I61">
-        <v>-3.717348722178685</v>
+        <v>-8.153728018412449</v>
       </c>
       <c r="J61">
         <v>0.7065714465111699</v>
@@ -2580,7 +2580,7 @@
         <v>32.57171806106061</v>
       </c>
       <c r="I62">
-        <v>-8.002577950508808</v>
+        <v>-8.237315139506272</v>
       </c>
       <c r="J62">
         <v>-0.8557952713669732</v>
@@ -2615,7 +2615,7 @@
         <v>22.57380177706742</v>
       </c>
       <c r="I63">
-        <v>-8.167096864782222</v>
+        <v>-8.572663828118074</v>
       </c>
       <c r="J63">
         <v>1.916084051494495</v>
@@ -2650,7 +2650,7 @@
         <v>27.28275405335008</v>
       </c>
       <c r="I64">
-        <v>-9.553104276730711</v>
+        <v>-7.905843949948903</v>
       </c>
       <c r="J64">
         <v>-0.9815813158366428</v>
@@ -2685,7 +2685,7 @@
         <v>25.95568133519952</v>
       </c>
       <c r="I65">
-        <v>-8.583058365037582</v>
+        <v>-7.743217249034733</v>
       </c>
       <c r="J65">
         <v>0.1869801932320439</v>
@@ -2720,7 +2720,7 @@
         <v>23.17815197721138</v>
       </c>
       <c r="I66">
-        <v>-9.544003255257243</v>
+        <v>-8.053152202907722</v>
       </c>
       <c r="J66">
         <v>-0.4534660573141888</v>
@@ -2755,7 +2755,7 @@
         <v>33.05322997450421</v>
       </c>
       <c r="I67">
-        <v>-6.778305861388696</v>
+        <v>-6.53676826507846</v>
       </c>
       <c r="J67">
         <v>0.01826837770696148</v>
@@ -2790,7 +2790,7 @@
         <v>36.96725425776677</v>
       </c>
       <c r="I68">
-        <v>-8.416766187042571</v>
+        <v>-8.632793407977031</v>
       </c>
       <c r="J68">
         <v>-2.41687525220319</v>
@@ -2825,7 +2825,7 @@
         <v>26.97137127111055</v>
       </c>
       <c r="I69">
-        <v>-9.619086871081018</v>
+        <v>-7.176267397421673</v>
       </c>
       <c r="J69">
         <v>0.5820827956595995</v>
@@ -2860,7 +2860,7 @@
         <v>39.64340850397054</v>
       </c>
       <c r="I70">
-        <v>-8.356410155875018</v>
+        <v>-8.49183100729838</v>
       </c>
       <c r="J70">
         <v>-3.011428351631623</v>
@@ -2895,7 +2895,7 @@
         <v>24.59314285714271</v>
       </c>
       <c r="I71">
-        <v>-8.449424444704068</v>
+        <v>-8.619264349490173</v>
       </c>
       <c r="J71">
         <v>1.924442052702609</v>
@@ -2930,7 +2930,7 @@
         <v>50.11636441212119</v>
       </c>
       <c r="I72">
-        <v>-5.209554339092263</v>
+        <v>-7.076943163223855</v>
       </c>
       <c r="J72">
         <v>-4.742309175156709</v>
@@ -2965,7 +2965,7 @@
         <v>39.05998080000573</v>
       </c>
       <c r="I73">
-        <v>2.75364932435731</v>
+        <v>-3.838751341060898</v>
       </c>
       <c r="J73">
         <v>0.1478812736530021</v>
@@ -3000,7 +3000,7 @@
         <v>29.78997119999549</v>
       </c>
       <c r="I74">
-        <v>-0.3432917684046545</v>
+        <v>-8.042601991578854</v>
       </c>
       <c r="J74">
         <v>-0.06540268445854228</v>
@@ -3035,7 +3035,7 @@
         <v>33.03006734789524</v>
       </c>
       <c r="I75">
-        <v>-2.163172582978273</v>
+        <v>-6.870141044036783</v>
       </c>
       <c r="J75">
         <v>0.09262105779320534</v>
@@ -3070,7 +3070,7 @@
         <v>33.20883752336142</v>
       </c>
       <c r="I76">
-        <v>-7.400348837974517</v>
+        <v>-8.619094840519754</v>
       </c>
       <c r="J76">
         <v>-0.6315796728633352</v>
@@ -3105,7 +3105,7 @@
         <v>16.26989971200004</v>
       </c>
       <c r="I77">
-        <v>-7.395155115602038</v>
+        <v>-6.3383900335262</v>
       </c>
       <c r="J77">
         <v>2.716089318916377</v>
@@ -3140,7 +3140,7 @@
         <v>24.62401875087118</v>
       </c>
       <c r="I78">
-        <v>-9.222611481229899</v>
+        <v>18.04830815444006</v>
       </c>
       <c r="J78">
         <v>-2.89897968096449</v>
@@ -3175,7 +3175,7 @@
         <v>17.94454551151508</v>
       </c>
       <c r="I79">
-        <v>-4.616251977627688</v>
+        <v>-2.446379725814278</v>
       </c>
       <c r="J79">
         <v>3.320842647314708</v>
@@ -3210,7 +3210,7 @@
         <v>30.91946620618353</v>
       </c>
       <c r="I80">
-        <v>5.634233386028945</v>
+        <v>-20.54843681064228</v>
       </c>
       <c r="J80">
         <v>-2.378381178288861</v>
@@ -3245,7 +3245,7 @@
         <v>34.55984194861541</v>
       </c>
       <c r="I81">
-        <v>-5.182002164789509</v>
+        <v>-9.884981934753164</v>
       </c>
       <c r="J81">
         <v>0.5020928043205873</v>
@@ -3280,7 +3280,7 @@
         <v>32.91375362058016</v>
       </c>
       <c r="I82">
-        <v>-6.027292811915447</v>
+        <v>-10.70401572749789</v>
       </c>
       <c r="J82">
         <v>-0.0403003273372541</v>
@@ -3315,7 +3315,7 @@
         <v>33.10587218336364</v>
       </c>
       <c r="I83">
-        <v>-5.336842640111707</v>
+        <v>-9.134661075365083</v>
       </c>
       <c r="J83">
         <v>0.04951041999931714</v>
@@ -3350,7 +3350,7 @@
         <v>38.66532171090319</v>
       </c>
       <c r="I84">
-        <v>5.370848507319992</v>
+        <v>-9.040074013974287</v>
       </c>
       <c r="J84">
         <v>-2.011361822874231</v>
@@ -3385,7 +3385,7 @@
         <v>28.34591219069054</v>
       </c>
       <c r="I85">
-        <v>9.371499734292753</v>
+        <v>-6.032804544250584</v>
       </c>
       <c r="J85">
         <v>1.463991527515775</v>
@@ -3420,7 +3420,7 @@
         <v>37.86786386771843</v>
       </c>
       <c r="I86">
-        <v>9.540074389962008</v>
+        <v>-7.463632910074563</v>
       </c>
       <c r="J86">
         <v>-2.655849040250382</v>
@@ -3455,7 +3455,7 @@
         <v>39.3439600683123</v>
       </c>
       <c r="I87">
-        <v>9.837276853847781</v>
+        <v>-7.966799200593401</v>
       </c>
       <c r="J87">
         <v>0.2346998995295671</v>
@@ -3490,7 +3490,7 @@
         <v>41.5449891173261</v>
       </c>
       <c r="I88">
-        <v>8.286061890166851</v>
+        <v>-2.4672570562392</v>
       </c>
       <c r="J88">
         <v>-2.203548292072909</v>
@@ -3525,7 +3525,7 @@
         <v>20.06356539795187</v>
       </c>
       <c r="I89">
-        <v>5.380482186853995</v>
+        <v>4.464205068425484</v>
       </c>
       <c r="J89">
         <v>4.210450035293675</v>
@@ -3560,7 +3560,7 @@
         <v>35.64995883891307</v>
       </c>
       <c r="I90">
-        <v>8.415171640824887</v>
+        <v>-1.154930704642829</v>
       </c>
       <c r="J90">
         <v>-2.202256155180089</v>
@@ -3595,7 +3595,7 @@
         <v>22.75865569454824</v>
       </c>
       <c r="I91">
-        <v>8.530625284888545</v>
+        <v>-1.632373324031598</v>
       </c>
       <c r="J91">
         <v>3.050741786215558</v>
@@ -3630,7 +3630,7 @@
         <v>30.49486013079875</v>
       </c>
       <c r="I92">
-        <v>9.203217601977194</v>
+        <v>-4.386073801690693</v>
       </c>
       <c r="J92">
         <v>-0.3811257289983556</v>
@@ -3665,7 +3665,7 @@
         <v>16.3955298087464</v>
       </c>
       <c r="I93">
-        <v>9.49989785175754</v>
+        <v>-8.911496991078922</v>
       </c>
       <c r="J93">
         <v>2.225124291033696</v>
@@ -3700,7 +3700,7 @@
         <v>27.34172248563368</v>
       </c>
       <c r="I94">
-        <v>9.790242349974314</v>
+        <v>-9.602777963159939</v>
       </c>
       <c r="J94">
         <v>-0.6709616516872338</v>
@@ -3735,7 +3735,7 @@
         <v>22.42451012446292</v>
       </c>
       <c r="I95">
-        <v>8.723912600517865</v>
+        <v>-20.04425436588004</v>
       </c>
       <c r="J95">
         <v>2.698331378401192</v>
@@ -3770,7 +3770,7 @@
         <v>39.59784603492827</v>
       </c>
       <c r="I96">
-        <v>7.298317747979256</v>
+        <v>-20.42575044167924</v>
       </c>
       <c r="J96">
         <v>-3.708417131282641</v>
@@ -3805,7 +3805,7 @@
         <v>29.59116748241858</v>
       </c>
       <c r="I97">
-        <v>9.096321182631511</v>
+        <v>-19.4612149960238</v>
       </c>
       <c r="J97">
         <v>1.634751196220996</v>
@@ -3840,7 +3840,7 @@
         <v>36.4276932339744</v>
       </c>
       <c r="I98">
-        <v>4.931120912629898</v>
+        <v>-21.64114728075592</v>
       </c>
       <c r="J98">
         <v>-0.6483560142127298</v>
@@ -3875,7 +3875,7 @@
         <v>26.89666854402325</v>
       </c>
       <c r="I99">
-        <v>8.241120482499934</v>
+        <v>-21.14844450982296</v>
       </c>
       <c r="J99">
         <v>1.445689524402347</v>
@@ -3910,7 +3910,7 @@
         <v>36.06929483897707</v>
       </c>
       <c r="I100">
-        <v>8.822678308569643</v>
+        <v>-17.62083010164855</v>
       </c>
       <c r="J100">
         <v>-0.9708495266484006</v>
@@ -3945,7 +3945,7 @@
         <v>36.09623736751487</v>
       </c>
       <c r="I101">
-        <v>9.715138701987225</v>
+        <v>-16.51826334882265</v>
       </c>
       <c r="J101">
         <v>0.5361296906775379</v>
@@ -3980,7 +3980,7 @@
         <v>40.55228609883108</v>
       </c>
       <c r="I102">
-        <v>7.343718501274182</v>
+        <v>-18.39629186669524</v>
       </c>
       <c r="J102">
         <v>-1.306916924161506</v>
@@ -4015,7 +4015,7 @@
         <v>34.65471384827193</v>
       </c>
       <c r="I103">
-        <v>1.203375422079021</v>
+        <v>-20.80302228232813</v>
       </c>
       <c r="J103">
         <v>0.4606134820140909</v>
@@ -4050,7 +4050,7 @@
         <v>35.08972199202882</v>
       </c>
       <c r="I104">
-        <v>1.174032653567299</v>
+        <v>-19.30971753996017</v>
       </c>
       <c r="J104">
         <v>-0.1927582801566693</v>
@@ -4085,7 +4085,7 @@
         <v>24.51064049097011</v>
       </c>
       <c r="I105">
-        <v>-0.2475810672386195</v>
+        <v>-14.56170605756262</v>
       </c>
       <c r="J105">
         <v>2.655858088192967</v>
@@ -4120,7 +4120,7 @@
         <v>36.77868544697363</v>
       </c>
       <c r="I106">
-        <v>9.288306386557462</v>
+        <v>-18.73622465458683</v>
       </c>
       <c r="J106">
         <v>-2.375986148529549</v>
@@ -4155,7 +4155,7 @@
         <v>21.86689850030181</v>
       </c>
       <c r="I107">
-        <v>-1.995007604916941</v>
+        <v>-9.069783058316565</v>
       </c>
       <c r="J107">
         <v>1.607190827481332</v>
@@ -4190,7 +4190,7 @@
         <v>32.78570770277357</v>
       </c>
       <c r="I108">
-        <v>4.042399394869451</v>
+        <v>-21.04926322567263</v>
       </c>
       <c r="J108">
         <v>-1.506333985786823</v>
@@ -4225,7 +4225,7 @@
         <v>24.52320061444814</v>
       </c>
       <c r="I109">
-        <v>9.86363780367706</v>
+        <v>-17.45340994417572</v>
       </c>
       <c r="J109">
         <v>1.300215303882292</v>
@@ -4260,7 +4260,7 @@
         <v>39.58432026256865</v>
       </c>
       <c r="I110">
-        <v>9.611461288350222</v>
+        <v>-10.27951649280293</v>
       </c>
       <c r="J110">
         <v>-1.850920936461603</v>
@@ -4295,7 +4295,7 @@
         <v>23.75197917772135</v>
       </c>
       <c r="I111">
-        <v>8.41242255882405</v>
+        <v>-1.09812700803578</v>
       </c>
       <c r="J111">
         <v>1.850824805204204</v>
@@ -4330,7 +4330,7 @@
         <v>34.267817244218</v>
       </c>
       <c r="I112">
-        <v>9.092899302756813</v>
+        <v>-5.35344681787933</v>
       </c>
       <c r="J112">
         <v>-0.8437171519583012</v>
@@ -4365,7 +4365,7 @@
         <v>29.73466625705987</v>
       </c>
       <c r="I113">
-        <v>7.073828968541319</v>
+        <v>3.263925216724501</v>
       </c>
       <c r="J113">
         <v>0.5620954464370019</v>
@@ -4400,7 +4400,7 @@
         <v>30.09320076445947</v>
       </c>
       <c r="I114">
-        <v>9.572132577961794</v>
+        <v>-5.649520336079888</v>
       </c>
       <c r="J114">
         <v>-0.1079889486437517</v>
@@ -4435,7 +4435,7 @@
         <v>34.56719127666147</v>
       </c>
       <c r="I115">
-        <v>8.420851211849275</v>
+        <v>-6.027853670577458</v>
       </c>
       <c r="J115">
         <v>0.08442155832973504</v>
@@ -4470,7 +4470,7 @@
         <v>30.6</v>
       </c>
       <c r="I116">
-        <v>8.085686616646532</v>
+        <v>-5.825958835778462</v>
       </c>
       <c r="J116">
         <v>-0.007052218041494866</v>
@@ -4505,7 +4505,7 @@
         <v>29.97599894151136</v>
       </c>
       <c r="I117">
-        <v>10.06847942874839</v>
+        <v>-7.640955813495007</v>
       </c>
       <c r="J117">
         <v>0.06800232979748784</v>
@@ -4540,7 +4540,7 @@
         <v>30.40472212029054</v>
       </c>
       <c r="I118">
-        <v>9.271978773966771</v>
+        <v>-6.872030612441593</v>
       </c>
       <c r="J118">
         <v>-0.05033214386252345</v>
@@ -4575,7 +4575,7 @@
         <v>33.52856395356066</v>
       </c>
       <c r="I119">
-        <v>7.865691904854045</v>
+        <v>-5.871115914526712</v>
       </c>
       <c r="J119">
         <v>0.03682857583051144</v>
@@ -4610,7 +4610,7 @@
         <v>28.28221104038536</v>
       </c>
       <c r="I120">
-        <v>9.7873247852002</v>
+        <v>-11.90563661051357</v>
       </c>
       <c r="J120">
         <v>-0.5522155183379623</v>
@@ -4645,7 +4645,7 @@
         <v>22.55536433015659</v>
       </c>
       <c r="I121">
-        <v>13.69439617394468</v>
+        <v>-21.61862857643989</v>
       </c>
       <c r="J121">
         <v>0.01630727778432586</v>
@@ -4680,7 +4680,7 @@
         <v>26.57378476293161</v>
       </c>
       <c r="I122">
-        <v>9.798239447465125</v>
+        <v>-15.39462585008512</v>
       </c>
       <c r="J122">
         <v>-0.1581156589084742</v>
@@ -4715,7 +4715,7 @@
         <v>20.95358828449676</v>
       </c>
       <c r="I123">
-        <v>9.527133510341967</v>
+        <v>-14.48580125649026</v>
       </c>
       <c r="J123">
         <v>2.734520020551302</v>
@@ -4750,7 +4750,7 @@
         <v>25.41148110697468</v>
       </c>
       <c r="I124">
-        <v>9.455939329390315</v>
+        <v>-9.152576896830869</v>
       </c>
       <c r="J124">
         <v>-0.1462926043532186</v>
@@ -4785,7 +4785,7 @@
         <v>26.28266630257325</v>
       </c>
       <c r="I125">
-        <v>9.965924621837534</v>
+        <v>-12.92829670078912</v>
       </c>
       <c r="J125">
         <v>1.487885549059953</v>
@@ -4820,7 +4820,7 @@
         <v>32.72228400906096</v>
       </c>
       <c r="I126">
-        <v>10.05388797329462</v>
+        <v>-16.70010355190625</v>
       </c>
       <c r="J126">
         <v>-0.1633661034706355</v>
@@ -4855,7 +4855,7 @@
         <v>18.79271875091716</v>
       </c>
       <c r="I127">
-        <v>7.129905867911899</v>
+        <v>-6.355314490952775</v>
       </c>
       <c r="J127">
         <v>3.72633530593552</v>
@@ -4890,7 +4890,7 @@
         <v>27.46799088655971</v>
       </c>
       <c r="I128">
-        <v>8.180094064232685</v>
+        <v>-3.692080949066731</v>
       </c>
       <c r="J128">
         <v>-0.4547480249172512</v>
@@ -4925,7 +4925,7 @@
         <v>16.61000183672015</v>
       </c>
       <c r="I129">
-        <v>4.95770754844031</v>
+        <v>0.01192908277232559</v>
       </c>
       <c r="J129">
         <v>4.990099413684296</v>
@@ -4960,7 +4960,7 @@
         <v>44.51245009901432</v>
       </c>
       <c r="I130">
-        <v>-6.050718766824447</v>
+        <v>1.648637175470295</v>
       </c>
       <c r="J130">
         <v>-5.3247206802141</v>
@@ -4995,7 +4995,7 @@
         <v>1.718991550881645</v>
       </c>
       <c r="I131">
-        <v>-0.485295255565031</v>
+        <v>0.1625352366917141</v>
       </c>
       <c r="J131">
         <v>2.311267454374387</v>
@@ -5030,7 +5030,7 @@
         <v>52.82596571830113</v>
       </c>
       <c r="I132">
-        <v>-7.135060693235335</v>
+        <v>15.93059255803749</v>
       </c>
       <c r="J132">
         <v>-5.297177455155476</v>
@@ -5065,7 +5065,7 @@
         <v>18.82483367164588</v>
       </c>
       <c r="I133">
-        <v>-3.386490325455647</v>
+        <v>20.78183393235086</v>
       </c>
       <c r="J133">
         <v>1.835691384337092</v>
@@ -5100,7 +5100,7 @@
         <v>38.13103127647958</v>
       </c>
       <c r="I134">
-        <v>-9.678537165513065</v>
+        <v>17.35062716321346</v>
       </c>
       <c r="J134">
         <v>-3.184215986076885</v>
@@ -5135,7 +5135,7 @@
         <v>19.53490811777877</v>
       </c>
       <c r="I135">
-        <v>-7.822895136897515</v>
+        <v>17.67815589476014</v>
       </c>
       <c r="J135">
         <v>1.575641440105612</v>
@@ -5170,7 +5170,7 @@
         <v>22.50228628472001</v>
       </c>
       <c r="I136">
-        <v>-9.522569014343407</v>
+        <v>14.79292678370674</v>
       </c>
       <c r="J136">
         <v>-0.5184604842033844</v>
@@ -5205,7 +5205,7 @@
         <v>19.31760073728001</v>
       </c>
       <c r="I137">
-        <v>-7.938714052714205</v>
+        <v>21.0574410241931</v>
       </c>
       <c r="J137">
         <v>0.4350344343097402</v>
@@ -5240,7 +5240,7 @@
         <v>31.69306047749037</v>
       </c>
       <c r="I138">
-        <v>-9.453702425943769</v>
+        <v>17.96509081449862</v>
       </c>
       <c r="J138">
         <v>-3.838507784996027</v>
@@ -5275,7 +5275,7 @@
         <v>28.32146246144323</v>
       </c>
       <c r="I139">
-        <v>-9.484078331679129</v>
+        <v>16.94129946503948</v>
       </c>
       <c r="J139">
         <v>1.070528177159208</v>
@@ -5310,7 +5310,7 @@
         <v>20.39892089345085</v>
       </c>
       <c r="I140">
-        <v>-14.67691917690695</v>
+        <v>25.43773561540255</v>
       </c>
       <c r="J140">
         <v>-0.04873472114341066</v>
@@ -5345,7 +5345,7 @@
         <v>29.11254323958347</v>
       </c>
       <c r="I141">
-        <v>-9.199754894649987</v>
+        <v>15.52096834685122</v>
       </c>
       <c r="J141">
         <v>0.05220452022249678</v>
@@ -5380,7 +5380,7 @@
         <v>2.375886989165604</v>
       </c>
       <c r="I142">
-        <v>-4.215354252944962</v>
+        <v>15.22250054886092</v>
       </c>
       <c r="J142">
         <v>-0.670211768767337</v>
@@ -5415,7 +5415,7 @@
         <v>29.95250514749979</v>
       </c>
       <c r="I143">
-        <v>-5.11209443702188</v>
+        <v>23.03164817287215</v>
       </c>
       <c r="J143">
         <v>0.5454060938350256</v>
@@ -5450,7 +5450,7 @@
         <v>35.65413055798746</v>
       </c>
       <c r="I144">
-        <v>-4.614677363142945</v>
+        <v>22.45428720102987</v>
       </c>
       <c r="J144">
         <v>-1.63588619386972</v>
@@ -5485,7 +5485,7 @@
         <v>25.46257449064387</v>
       </c>
       <c r="I145">
-        <v>-2.427551876007942</v>
+        <v>21.12647855265024</v>
       </c>
       <c r="J145">
         <v>2.34855369988183</v>
@@ -5520,7 +5520,7 @@
         <v>39.58535843135407</v>
       </c>
       <c r="I146">
-        <v>-5.952883164023183</v>
+        <v>22.72867287059101</v>
       </c>
       <c r="J146">
         <v>-1.591479697216521</v>
@@ -5555,7 +5555,7 @@
         <v>31.7732159314542</v>
       </c>
       <c r="I147">
-        <v>-6.036582125376199</v>
+        <v>23.30563997228808</v>
       </c>
       <c r="J147">
         <v>0.8586559419295883</v>
@@ -5590,7 +5590,7 @@
         <v>33.06098007263697</v>
       </c>
       <c r="I148">
-        <v>-5.954165415930233</v>
+        <v>22.95501837837722</v>
       </c>
       <c r="J148">
         <v>-0.6032174954530958</v>
@@ -5625,7 +5625,7 @@
         <v>33.33321478749592</v>
       </c>
       <c r="I149">
-        <v>-5.873510929230008</v>
+        <v>22.58429153456347</v>
       </c>
       <c r="J149">
         <v>1.345029471545996</v>
@@ -5660,7 +5660,7 @@
         <v>38.14457773090822</v>
       </c>
       <c r="I150">
-        <v>-6.127458124228686</v>
+        <v>23.98935297734973</v>
       </c>
       <c r="J150">
         <v>-0.1746349332992998</v>
@@ -5695,7 +5695,7 @@
         <v>32.08045441558721</v>
       </c>
       <c r="I151">
-        <v>-4.630134846299257</v>
+        <v>21.1226940996934</v>
       </c>
       <c r="J151">
         <v>1.848148279983113</v>
@@ -5730,7 +5730,7 @@
         <v>44.98130829103623</v>
       </c>
       <c r="I152">
-        <v>-8.191103671117139</v>
+        <v>21.1719270110728</v>
       </c>
       <c r="J152">
         <v>-2.8988323384235</v>
@@ -5765,7 +5765,7 @@
         <v>40.19400184328843</v>
       </c>
       <c r="I153">
-        <v>-9.872602979078311</v>
+        <v>16.83560174043009</v>
       </c>
       <c r="J153">
         <v>0.3548845399372224</v>
@@ -5800,7 +5800,7 @@
         <v>38.41182397764351</v>
       </c>
       <c r="I154">
-        <v>-8.161969047703799</v>
+        <v>13.66618299841011</v>
       </c>
       <c r="J154">
         <v>-0.03395882347243673</v>
@@ -5835,7 +5835,7 @@
         <v>34.34799416251772</v>
       </c>
       <c r="I155">
-        <v>-1.278984264475624</v>
+        <v>16.85305791803759</v>
       </c>
       <c r="J155">
         <v>0.1693939310309182</v>
@@ -5870,7 +5870,7 @@
         <v>41.75101872725513</v>
       </c>
       <c r="I156">
-        <v>-7.644398633726552</v>
+        <v>22.23873953780762</v>
       </c>
       <c r="J156">
         <v>-1.073403658806128</v>
@@ -5905,7 +5905,7 @@
         <v>41.30383793354189</v>
       </c>
       <c r="I157">
-        <v>-7.48113694021511</v>
+        <v>21.74477309104083</v>
       </c>
       <c r="J157">
         <v>0.2809075621413292</v>
@@ -5940,7 +5940,7 @@
         <v>38.7235377171688</v>
       </c>
       <c r="I158">
-        <v>-6.556918697489641</v>
+        <v>20.16157165876046</v>
       </c>
       <c r="J158">
         <v>-0.4089173317273982</v>
@@ -5975,7 +5975,7 @@
         <v>36.54505585098669</v>
       </c>
       <c r="I159">
-        <v>-6.918059535906386</v>
+        <v>26.69948500421053</v>
       </c>
       <c r="J159">
         <v>0.07642526339900327</v>
@@ -6010,7 +6010,7 @@
         <v>39.55328772676476</v>
       </c>
       <c r="I160">
-        <v>-7.310950032612866</v>
+        <v>22.2419116406103</v>
       </c>
       <c r="J160">
         <v>-1.976720580193494</v>
@@ -6045,7 +6045,7 @@
         <v>25.7840528862269</v>
       </c>
       <c r="I161">
-        <v>-7.260213916256795</v>
+        <v>21.73104603758204</v>
       </c>
       <c r="J161">
         <v>2.01497177180718</v>
@@ -6080,7 +6080,7 @@
         <v>24.61980032256019</v>
       </c>
       <c r="I162">
-        <v>-6.617649075004772</v>
+        <v>21.10146710313327</v>
       </c>
       <c r="J162">
         <v>-1.029021790149003</v>
@@ -6115,7 +6115,7 @@
         <v>23.29934495204999</v>
       </c>
       <c r="I163">
-        <v>-6.188022093418824</v>
+        <v>22.55609008091706</v>
       </c>
       <c r="J163">
         <v>2.685890804089419</v>
@@ -6150,7 +6150,7 @@
         <v>30.16831767479889</v>
       </c>
       <c r="I164">
-        <v>-2.64405516230874</v>
+        <v>21.01830242266158</v>
       </c>
       <c r="J164">
         <v>-0.147749617076826</v>
@@ -6185,7 +6185,7 @@
         <v>18.68682259732583</v>
       </c>
       <c r="I165">
-        <v>-8.060322037523719</v>
+        <v>18.63295584543046</v>
       </c>
       <c r="J165">
         <v>3.909868058315815</v>
@@ -6220,7 +6220,7 @@
         <v>37.38188659446314</v>
       </c>
       <c r="I166">
-        <v>-8.511190228102087</v>
+        <v>15.05583196812712</v>
       </c>
       <c r="J166">
         <v>-0.1088162155565466</v>
@@ -6255,7 +6255,7 @@
         <v>14.06264363495939</v>
       </c>
       <c r="I167">
-        <v>-9.529733878857352</v>
+        <v>16.52905192663678</v>
       </c>
       <c r="J167">
         <v>5.452839610222722</v>
@@ -6290,7 +6290,7 @@
         <v>43.41793073966569</v>
       </c>
       <c r="I168">
-        <v>0.09371724543532153</v>
+        <v>-11.89973300784589</v>
       </c>
       <c r="J168">
         <v>-5.83065103627928</v>
@@ -6325,7 +6325,7 @@
         <v>32.32430686301579</v>
       </c>
       <c r="I169">
-        <v>-9.797943347235737</v>
+        <v>9.364415498571526</v>
       </c>
       <c r="J169">
         <v>0.2446934562775982</v>
@@ -6360,7 +6360,7 @@
         <v>40.67585245164467</v>
       </c>
       <c r="I170">
-        <v>-6.278024187698132</v>
+        <v>-2.394237261393395</v>
       </c>
       <c r="J170">
         <v>-2.298993753856324</v>
@@ -6395,7 +6395,7 @@
         <v>41.8589301425399</v>
       </c>
       <c r="I171">
-        <v>-9.981710438881915</v>
+        <v>13.5294655965551</v>
       </c>
       <c r="J171">
         <v>0.142538583395602</v>
@@ -6430,7 +6430,7 @@
         <v>48.35324379889026</v>
       </c>
       <c r="I172">
-        <v>-0.5608130625028831</v>
+        <v>-14.8768808997706</v>
       </c>
       <c r="J172">
         <v>-3.418624920076051</v>
@@ -6465,7 +6465,7 @@
         <v>29.45646408273948</v>
       </c>
       <c r="I173">
-        <v>-4.525243210382761</v>
+        <v>-10.78024896390646</v>
       </c>
       <c r="J173">
         <v>0.1890365598188715</v>
@@ -6500,7 +6500,7 @@
         <v>31.2820004096051</v>
       </c>
       <c r="I174">
-        <v>-0.6325978247313008</v>
+        <v>-15.57524507831555</v>
       </c>
       <c r="J174">
         <v>-1.068537812006906</v>
@@ -6535,7 +6535,7 @@
         <v>26.12541480060172</v>
       </c>
       <c r="I175">
-        <v>1.066671473496194</v>
+        <v>-17.09980432958485</v>
       </c>
       <c r="J175">
         <v>1.631311670923605</v>
@@ -6570,7 +6570,7 @@
         <v>29.23399979520036</v>
       </c>
       <c r="I176">
-        <v>-4.873796282460561</v>
+        <v>-4.606888659310218</v>
       </c>
       <c r="J176">
         <v>-0.9007381798634719</v>
@@ -6605,7 +6605,7 @@
         <v>20.95783095995479</v>
       </c>
       <c r="I177">
-        <v>-9.275599690914749</v>
+        <v>5.853415243864639</v>
       </c>
       <c r="J177">
         <v>2.345938395948998</v>
@@ -6640,7 +6640,7 @@
         <v>23.9744336270378</v>
       </c>
       <c r="I178">
-        <v>-11.61063315747984</v>
+        <v>9.123086206092713</v>
       </c>
       <c r="J178">
         <v>-0.01951837058685416</v>
@@ -6675,7 +6675,7 @@
         <v>28.95845868755132</v>
       </c>
       <c r="I179">
-        <v>-11.13584095399499</v>
+        <v>7.604685693915659</v>
       </c>
       <c r="J179">
         <v>0.1749480088949199</v>
@@ -6710,7 +6710,7 @@
         <v>32.47332599490971</v>
       </c>
       <c r="I180">
-        <v>-8.398006233318581</v>
+        <v>1.441542295161181</v>
       </c>
       <c r="J180">
         <v>-1.018714615424635</v>
@@ -6745,7 +6745,7 @@
         <v>25.53480036864721</v>
       </c>
       <c r="I181">
-        <v>-8.157451075802864</v>
+        <v>0.6225464125393471</v>
       </c>
       <c r="J181">
         <v>1.476624928275096</v>
@@ -6780,7 +6780,7 @@
         <v>39.76503074560448</v>
       </c>
       <c r="I182">
-        <v>-8.716814630915582</v>
+        <v>2.41516849582244</v>
       </c>
       <c r="J182">
         <v>-2.383206386767698</v>
@@ -6815,7 +6815,7 @@
         <v>28.77631917270042</v>
       </c>
       <c r="I183">
-        <v>-7.667586426570379</v>
+        <v>-1.408598463358226</v>
       </c>
       <c r="J183">
         <v>1.996910454996203</v>
@@ -6850,7 +6850,7 @@
         <v>33.37395199849932</v>
       </c>
       <c r="I184">
-        <v>-9.274327655751529</v>
+        <v>5.448286983529887</v>
       </c>
       <c r="J184">
         <v>-0.7693198050873349</v>
@@ -6885,7 +6885,7 @@
         <v>28.16345460130939</v>
       </c>
       <c r="I185">
-        <v>-8.520384411470172</v>
+        <v>1.585481854138689</v>
       </c>
       <c r="J185">
         <v>1.199605133267401</v>
@@ -6920,7 +6920,7 @@
         <v>38.20926052250464</v>
       </c>
       <c r="I186">
-        <v>-9.349785935545057</v>
+        <v>6.194359202766951</v>
       </c>
       <c r="J186">
         <v>-2.291879511680342</v>
@@ -6955,7 +6955,7 @@
         <v>24.84787057826545</v>
       </c>
       <c r="I187">
-        <v>-7.511198645169115</v>
+        <v>-2.166430161217149</v>
       </c>
       <c r="J187">
         <v>2.536900337775251</v>
@@ -6990,7 +6990,7 @@
         <v>44.63200495858473</v>
       </c>
       <c r="I188">
-        <v>-8.685416039010645</v>
+        <v>4.912402266863766</v>
       </c>
       <c r="J188">
         <v>-3.843987814466523</v>
@@ -7025,7 +7025,7 @@
         <v>27.55454777408741</v>
       </c>
       <c r="I189">
-        <v>-4.480743662744738</v>
+        <v>-9.217996422946658</v>
       </c>
       <c r="J189">
         <v>2.996649237280884</v>
@@ -7060,7 +7060,7 @@
         <v>36.05291175211491</v>
       </c>
       <c r="I190">
-        <v>-2.465296216544731</v>
+        <v>-10.95092741486225</v>
       </c>
       <c r="J190">
         <v>-1.333681040377988</v>
@@ -7095,7 +7095,7 @@
         <v>25.4592169197427</v>
       </c>
       <c r="I191">
-        <v>-9.215912423138144</v>
+        <v>5.95936442417521</v>
       </c>
       <c r="J191">
         <v>1.822192976966776</v>
@@ -7130,7 +7130,7 @@
         <v>45.78794885407945</v>
       </c>
       <c r="I192">
-        <v>-9.580543900663962</v>
+        <v>7.800543222437926</v>
       </c>
       <c r="J192">
         <v>-3.578462665929078</v>
@@ -7165,7 +7165,7 @@
         <v>36.75610602017608</v>
       </c>
       <c r="I193">
-        <v>-9.630140881447478</v>
+        <v>8.561477044686249</v>
       </c>
       <c r="J193">
         <v>1.451388502985721</v>
@@ -7200,7 +7200,7 @@
         <v>45.62256619582649</v>
       </c>
       <c r="I194">
-        <v>-7.891974259445639</v>
+        <v>0.4589039636417902</v>
       </c>
       <c r="J194">
         <v>-2.722178330301135</v>
@@ -7235,7 +7235,7 @@
         <v>27.10435194360117</v>
       </c>
       <c r="I195">
-        <v>-5.398169116379909</v>
+        <v>-8.443080553415918</v>
       </c>
       <c r="J195">
         <v>1.202380712404819</v>
@@ -7270,7 +7270,7 @@
         <v>36.07320343945716</v>
       </c>
       <c r="I196">
-        <v>-5.400296802189629</v>
+        <v>-7.411638249817245</v>
       </c>
       <c r="J196">
         <v>-2.557812063154315</v>
@@ -7305,7 +7305,7 @@
         <v>39.6</v>
       </c>
       <c r="I197">
-        <v>-4.876966916489291</v>
+        <v>-9.877503872449187</v>
       </c>
       <c r="J197">
         <v>0.06636868731391132</v>
@@ -7340,7 +7340,7 @@
         <v>40.38086631514265</v>
       </c>
       <c r="I198">
-        <v>-5.872956654104112</v>
+        <v>-7.236401365158865</v>
       </c>
       <c r="J198">
         <v>-0.7839100865013273</v>
@@ -7375,7 +7375,7 @@
         <v>32.68500473879976</v>
       </c>
       <c r="I199">
-        <v>-7.963546826566753</v>
+        <v>-6.959538500924934</v>
       </c>
       <c r="J199">
         <v>0.02826293758782347</v>
@@ -7410,7 +7410,7 @@
         <v>40.40835641040467</v>
       </c>
       <c r="I200">
-        <v>-6.91389110936648</v>
+        <v>-6.200561116889467</v>
       </c>
       <c r="J200">
         <v>-0.147209116013751</v>
@@ -7445,7 +7445,7 @@
         <v>48.87733804917661</v>
       </c>
       <c r="I201">
-        <v>-3.901368018014115</v>
+        <v>-3.927460163151493</v>
       </c>
       <c r="J201">
         <v>0.008830890177810366</v>
@@ -7480,7 +7480,7 @@
         <v>38.90251900800067</v>
       </c>
       <c r="I202">
-        <v>-6.680159523634571</v>
+        <v>-5.821957744865879</v>
       </c>
       <c r="J202">
         <v>-0.2465507054419711</v>
@@ -7515,7 +7515,7 @@
         <v>35.51008467224285</v>
       </c>
       <c r="I203">
-        <v>0.4422984986050665</v>
+        <v>-11.80802776860332</v>
       </c>
       <c r="J203">
         <v>0.371854864864792</v>
@@ -7550,7 +7550,7 @@
         <v>31.66088677758481</v>
       </c>
       <c r="I204">
-        <v>10.00307007012053</v>
+        <v>-14.88796512389674</v>
       </c>
       <c r="J204">
         <v>-1.817381000673727</v>
@@ -7585,7 +7585,7 @@
         <v>37.50151520880754</v>
       </c>
       <c r="I205">
-        <v>7.102613810806504</v>
+        <v>-8.86269324953154</v>
       </c>
       <c r="J205">
         <v>0.01859062844219089</v>
@@ -7620,7 +7620,7 @@
         <v>37.59550716887632</v>
       </c>
       <c r="I206">
-        <v>8.766625765654869</v>
+        <v>-19.40423264060275</v>
       </c>
       <c r="J206">
         <v>-3.47640344105403</v>
@@ -7655,7 +7655,7 @@
         <v>20.92329966808947</v>
       </c>
       <c r="I207">
-        <v>8.20108571019291</v>
+        <v>-20.38575516473201</v>
       </c>
       <c r="J207">
         <v>1.656057392919211</v>
@@ -7690,7 +7690,7 @@
         <v>24.04246685538462</v>
       </c>
       <c r="I208">
-        <v>6.971313138636808</v>
+        <v>5.25946955305469</v>
       </c>
       <c r="J208">
         <v>-1.406857830386805</v>
@@ -7725,7 +7725,7 @@
         <v>23.62199917714285</v>
       </c>
       <c r="I209">
-        <v>6.046453057905566</v>
+        <v>4.419858597496508</v>
       </c>
       <c r="J209">
         <v>2.512540654681767</v>
@@ -7760,7 +7760,7 @@
         <v>28.8</v>
       </c>
       <c r="I210">
-        <v>7.090711575849358</v>
+        <v>5.502116176493622</v>
       </c>
       <c r="J210">
         <v>-0.2440415234351197</v>
@@ -7795,7 +7795,7 @@
         <v>27</v>
       </c>
       <c r="I211">
-        <v>8.290912066271199</v>
+        <v>6.617397042401089</v>
       </c>
       <c r="J211">
         <v>0.0225887839292227</v>
@@ -7830,7 +7830,7 @@
         <v>20.4</v>
       </c>
       <c r="I212">
-        <v>6.893780957924196</v>
+        <v>5.677158698603627</v>
       </c>
       <c r="J212">
         <v>-0.1421487722910462</v>
@@ -7865,7 +7865,7 @@
         <v>22.56585365853659</v>
       </c>
       <c r="I213">
-        <v>-2.650341406220098</v>
+        <v>-3.844939871296388</v>
       </c>
       <c r="J213">
         <v>2.552640772228497</v>
@@ -7900,7 +7900,7 @@
         <v>32.65714285714286</v>
       </c>
       <c r="I214">
-        <v>-8.309484016130456</v>
+        <v>-9.064658831552279</v>
       </c>
       <c r="J214">
         <v>-1.186858688947663</v>
@@ -7935,7 +7935,7 @@
         <v>27.78591549295775</v>
       </c>
       <c r="I215">
-        <v>1.470756713644611</v>
+        <v>-0.07203345948201248</v>
       </c>
       <c r="J215">
         <v>0.9284884428594385</v>
@@ -7970,7 +7970,7 @@
         <v>37.71692307692308</v>
       </c>
       <c r="I216">
-        <v>1.267028973438316</v>
+        <v>-0.6628807385995346</v>
       </c>
       <c r="J216">
         <v>-1.305567287382789</v>
@@ -8005,7 +8005,7 @@
         <v>34.77073170731708</v>
       </c>
       <c r="I217">
-        <v>4.380602489423286</v>
+        <v>2.603487623726155</v>
       </c>
       <c r="J217">
         <v>0.1455504403616825</v>
@@ -8040,7 +8040,7 @@
         <v>64.8</v>
       </c>
       <c r="I218">
-        <v>6.240439723534583</v>
+        <v>4.466675355966327</v>
       </c>
       <c r="J218">
         <v>-0.05817885455346388</v>
@@ -8075,7 +8075,7 @@
         <v>29.66170212765958</v>
       </c>
       <c r="I219">
-        <v>5.643840563560527</v>
+        <v>3.949750643986878</v>
       </c>
       <c r="J219">
         <v>1.34270425337591</v>
@@ -8110,7 +8110,7 @@
         <v>36.61334186666669</v>
       </c>
       <c r="I220">
-        <v>5.689910344931388</v>
+        <v>4.075700013613099</v>
       </c>
       <c r="J220">
         <v>-1.058893859008194</v>
@@ -8145,7 +8145,7 @@
         <v>24.339199488</v>
       </c>
       <c r="I221">
-        <v>7.629579425623613</v>
+        <v>6.381035392737139</v>
       </c>
       <c r="J221">
         <v>2.448574177348978</v>
@@ -8180,7 +8180,7 @@
         <v>29.87609542537048</v>
       </c>
       <c r="I222">
-        <v>6.586779733646623</v>
+        <v>5.184471429647139</v>
       </c>
       <c r="J222">
         <v>-0.7292787971415554</v>
@@ -8215,7 +8215,7 @@
         <v>18.18397991044832</v>
       </c>
       <c r="I223">
-        <v>7.236943948613054</v>
+        <v>6.184366378585902</v>
       </c>
       <c r="J223">
         <v>4.196090910036986</v>
@@ -8250,7 +8250,7 @@
         <v>25.08</v>
       </c>
       <c r="I224">
-        <v>6.682030506025773</v>
+        <v>5.852854270243405</v>
       </c>
       <c r="J224">
         <v>-0.5015807398417217</v>
@@ -8285,7 +8285,7 @@
         <v>18.54166666666667</v>
       </c>
       <c r="I225">
-        <v>-4.815998048643583</v>
+        <v>-6.11850894531086</v>
       </c>
       <c r="J225">
         <v>3.696612183854234</v>
@@ -8320,7 +8320,7 @@
         <v>29.63076923076923</v>
       </c>
       <c r="I226">
-        <v>9.470216725789474</v>
+        <v>8.600696455865357</v>
       </c>
       <c r="J226">
         <v>-0.1685148141837514</v>
@@ -8355,7 +8355,7 @@
         <v>22.84897959183673</v>
       </c>
       <c r="I227">
-        <v>-0.6804619097170322</v>
+        <v>-2.181659691475553</v>
       </c>
       <c r="J227">
         <v>2.647418303226958</v>
@@ -8390,7 +8390,7 @@
         <v>44.43037974683544</v>
       </c>
       <c r="I228">
-        <v>-9.571640250540145</v>
+        <v>-9.859140410258394</v>
       </c>
       <c r="J228">
         <v>-3.610825417008667</v>
@@ -8425,7 +8425,7 @@
         <v>21.68081632653061</v>
       </c>
       <c r="I229">
-        <v>-2.115841239722876</v>
+        <v>-3.265338002644624</v>
       </c>
       <c r="J229">
         <v>2.762792511049482</v>
@@ -8460,7 +8460,7 @@
         <v>32.26420247570618</v>
       </c>
       <c r="I230">
-        <v>-9.644727943817015</v>
+        <v>-9.036969631413456</v>
       </c>
       <c r="J230">
         <v>-0.8549666564867043</v>
@@ -8495,7 +8495,7 @@
         <v>31.14333384519778</v>
       </c>
       <c r="I231">
-        <v>-9.826852487895859</v>
+        <v>-9.172337575948717</v>
       </c>
       <c r="J231">
         <v>0.8276168795351351</v>
@@ -8530,7 +8530,7 @@
         <v>47.94756337972599</v>
       </c>
       <c r="I232">
-        <v>-9.162923090142227</v>
+        <v>-9.566352926965378</v>
       </c>
       <c r="J232">
         <v>-3.109755351085888</v>
@@ -8565,7 +8565,7 @@
         <v>18.86214302350518</v>
       </c>
       <c r="I233">
-        <v>-9.279721531126043</v>
+        <v>-9.437073007581498</v>
       </c>
       <c r="J233">
         <v>3.387199216937255</v>
@@ -8600,7 +8600,7 @@
         <v>25.2</v>
       </c>
       <c r="I234">
-        <v>-10.70818618231279</v>
+        <v>-10.3800331375912</v>
       </c>
       <c r="J234">
         <v>-0.07240085936359719</v>
@@ -8635,7 +8635,7 @@
         <v>27.9</v>
       </c>
       <c r="I235">
-        <v>-10.28083857050667</v>
+        <v>-9.855188399561477</v>
       </c>
       <c r="J235">
         <v>0.03438183632037943</v>
@@ -8670,7 +8670,7 @@
         <v>31.8</v>
       </c>
       <c r="I236">
-        <v>-10.69982126849787</v>
+        <v>-10.2356041880076</v>
       </c>
       <c r="J236">
         <v>-0.09267227944982946</v>
@@ -8705,7 +8705,7 @@
         <v>35.1</v>
       </c>
       <c r="I237">
-        <v>-9.70977966784228</v>
+        <v>-9.320317159286905</v>
       </c>
       <c r="J237">
         <v>0.02990053616783301</v>
@@ -8740,7 +8740,7 @@
         <v>41.09577464788732</v>
       </c>
       <c r="I238">
-        <v>-7.265834697397347</v>
+        <v>-7.746585718563649</v>
       </c>
       <c r="J238">
         <v>-2.695420036053109</v>
@@ -8775,7 +8775,7 @@
         <v>31.33333333333334</v>
       </c>
       <c r="I239">
-        <v>-5.434050553965608</v>
+        <v>-6.842704235058063</v>
       </c>
       <c r="J239">
         <v>0.2936775309057765</v>
@@ -8810,7 +8810,7 @@
         <v>34.89283236226419</v>
       </c>
       <c r="I240">
-        <v>-8.858105780211739</v>
+        <v>-9.396218669053013</v>
       </c>
       <c r="J240">
         <v>-0.5843724924823153</v>
@@ -8845,7 +8845,7 @@
         <v>32.57999556923068</v>
       </c>
       <c r="I241">
-        <v>-10.03166494985365</v>
+        <v>-10.13510455943811</v>
       </c>
       <c r="J241">
         <v>0.2746140251271925</v>
@@ -8880,7 +8880,7 @@
         <v>39.48480307199992</v>
       </c>
       <c r="I242">
-        <v>-9.77261975417392</v>
+        <v>-9.499364657580736</v>
       </c>
       <c r="J242">
         <v>-1.878127630907559</v>
@@ -8915,7 +8915,7 @@
         <v>29.80795392000117</v>
       </c>
       <c r="I243">
-        <v>-12.23179404362316</v>
+        <v>-12.79892932453439</v>
       </c>
       <c r="J243">
         <v>0.05269000990052013</v>
@@ -8950,7 +8950,7 @@
         <v>44.73391304347827</v>
       </c>
       <c r="I244">
-        <v>-6.704697597466803</v>
+        <v>-6.75361463899029</v>
       </c>
       <c r="J244">
         <v>-4.727483376833121</v>
@@ -8985,7 +8985,7 @@
         <v>19.61241685144124</v>
       </c>
       <c r="I245">
-        <v>-7.160339460142121</v>
+        <v>-7.368082007126756</v>
       </c>
       <c r="J245">
         <v>3.035195709746642</v>
@@ -9020,7 +9020,7 @@
         <v>37.00034581787227</v>
       </c>
       <c r="I246">
-        <v>-9.044504527580553</v>
+        <v>-9.225659214914405</v>
       </c>
       <c r="J246">
         <v>-2.353723003365933</v>
@@ -9055,7 +9055,7 @@
         <v>16.52340845114756</v>
       </c>
       <c r="I247">
-        <v>-9.130597484636958</v>
+        <v>-8.967490812360637</v>
       </c>
       <c r="J247">
         <v>4.766628259126644</v>
@@ -9090,7 +9090,7 @@
         <v>52.74044942071353</v>
       </c>
       <c r="I248">
-        <v>9.918384852875278</v>
+        <v>9.692974921972727</v>
       </c>
       <c r="J248">
         <v>-4.28486576279752</v>
@@ -9125,7 +9125,7 @@
         <v>29.61593099849573</v>
       </c>
       <c r="I249">
-        <v>9.223012588839298</v>
+        <v>9.663784113771865</v>
       </c>
       <c r="J249">
         <v>2.314130794988695</v>
@@ -9160,7 +9160,7 @@
         <v>42.69073170731708</v>
       </c>
       <c r="I250">
-        <v>6.942699997153567</v>
+        <v>7.078931701237821</v>
       </c>
       <c r="J250">
         <v>-3.191645510145635</v>
@@ -9195,7 +9195,7 @@
         <v>18.20083682008368</v>
       </c>
       <c r="I251">
-        <v>7.566191684677377</v>
+        <v>7.572948055286708</v>
       </c>
       <c r="J251">
         <v>4.056833265569304</v>
@@ -9230,7 +9230,7 @@
         <v>23.4</v>
       </c>
       <c r="I252">
-        <v>11.49689459563072</v>
+        <v>11.03203467863688</v>
       </c>
       <c r="J252">
         <v>-0.03493550885090931</v>
@@ -9265,7 +9265,7 @@
         <v>21.6</v>
       </c>
       <c r="I253">
-        <v>10.32671130665345</v>
+        <v>10.05328564321853</v>
       </c>
       <c r="J253">
         <v>0.03968028146535592</v>
@@ -9300,7 +9300,7 @@
         <v>32.12307692307692</v>
       </c>
       <c r="I254">
-        <v>9.739116832199027</v>
+        <v>9.924098368247888</v>
       </c>
       <c r="J254">
         <v>-0.1456951537468559</v>
@@ -9335,7 +9335,7 @@
         <v>28.8</v>
       </c>
       <c r="I255">
-        <v>9.703437845242144</v>
+        <v>9.92925680514292</v>
       </c>
       <c r="J255">
         <v>0.1115502650925748</v>
@@ -9370,7 +9370,7 @@
         <v>30</v>
       </c>
       <c r="I256">
-        <v>9.910880934115534</v>
+        <v>10.13049503098416</v>
       </c>
       <c r="J256">
         <v>-0.07432748377823373</v>
@@ -9405,7 +9405,7 @@
         <v>30.6</v>
       </c>
       <c r="I257">
-        <v>8.936070753066316</v>
+        <v>9.505250503780832</v>
       </c>
       <c r="J257">
         <v>0.8593211613760796</v>
@@ -9440,7 +9440,7 @@
         <v>34.2568481684209</v>
       </c>
       <c r="I258">
-        <v>6.554484847455418</v>
+        <v>7.613646098776196</v>
       </c>
       <c r="J258">
         <v>-0.5997305580630991</v>
@@ -9475,7 +9475,7 @@
         <v>21.31352031549298</v>
       </c>
       <c r="I259">
-        <v>7.615934940199608</v>
+        <v>7.997948314444776</v>
       </c>
       <c r="J259">
         <v>2.734965192807339</v>
@@ -9510,7 +9510,7 @@
         <v>46.95814389160361</v>
       </c>
       <c r="I260">
-        <v>9.204532501222005</v>
+        <v>9.381443017080942</v>
       </c>
       <c r="J260">
         <v>-3.27633981251283</v>
@@ -9545,7 +9545,7 @@
         <v>20.74245114991631</v>
       </c>
       <c r="I261">
-        <v>9.229589723639423</v>
+        <v>9.579856013711366</v>
       </c>
       <c r="J261">
         <v>3.130483564474789</v>
@@ -9580,7 +9580,7 @@
         <v>34.32</v>
       </c>
       <c r="I262">
-        <v>9.414014902130781</v>
+        <v>8.636977748368617</v>
       </c>
       <c r="J262">
         <v>-0.4176822975033736</v>
@@ -9615,7 +9615,7 @@
         <v>31.28143268571418</v>
       </c>
       <c r="I263">
-        <v>9.540800965604584</v>
+        <v>9.242909431232427</v>
       </c>
       <c r="J263">
         <v>0.9186658672281633</v>
@@ -9650,7 +9650,7 @@
         <v>36.24479539200011</v>
       </c>
       <c r="I264">
-        <v>9.22121326525426</v>
+        <v>9.548843469393869</v>
       </c>
       <c r="J264">
         <v>-2.140538234906929</v>
@@ -9685,7 +9685,7 @@
         <v>22.95</v>
       </c>
       <c r="I265">
-        <v>10.8696389217021</v>
+        <v>10.87549350582254</v>
       </c>
       <c r="J265">
         <v>0.1433745841357485</v>
@@ -9720,7 +9720,7 @@
         <v>42.14415104414355</v>
       </c>
       <c r="I266">
-        <v>-2.424028649325793</v>
+        <v>-0.9573820020241117</v>
       </c>
       <c r="J266">
         <v>-3.837102977199062</v>
@@ -9755,7 +9755,7 @@
         <v>40.28957731967967</v>
       </c>
       <c r="I267">
-        <v>-1.930643609826054</v>
+        <v>-0.2241183561436204</v>
       </c>
       <c r="J267">
         <v>0.1317364193051812</v>
@@ -9790,7 +9790,7 @@
         <v>46.14229446471911</v>
       </c>
       <c r="I268">
-        <v>2.968561236547542</v>
+        <v>4.257074360113119</v>
       </c>
       <c r="J268">
         <v>-2.184472475746754</v>
@@ -9825,7 +9825,7 @@
         <v>20.19208958537142</v>
       </c>
       <c r="I269">
-        <v>9.493078856341791</v>
+        <v>9.805988577521219</v>
       </c>
       <c r="J269">
         <v>3.739678310717578</v>
@@ -9860,7 +9860,7 @@
         <v>46.73080878545452</v>
       </c>
       <c r="I270">
-        <v>-1.362274464131487</v>
+        <v>0.1555101238874018</v>
       </c>
       <c r="J270">
         <v>-2.266873164493981</v>
@@ -9895,7 +9895,7 @@
         <v>37.04554758323939</v>
       </c>
       <c r="I271">
-        <v>-7.280902560806137</v>
+        <v>-5.644108533123892</v>
       </c>
       <c r="J271">
         <v>0.090943765837829</v>
@@ -9930,7 +9930,7 @@
         <v>49.7542176366466</v>
       </c>
       <c r="I272">
-        <v>5.168748717823248</v>
+        <v>6.465390340148595</v>
       </c>
       <c r="J272">
         <v>-3.824228518907837</v>
@@ -9965,7 +9965,7 @@
         <v>26.47</v>
       </c>
       <c r="I273">
-        <v>2.847610750739498</v>
+        <v>4.361549652176263</v>
       </c>
       <c r="J273">
         <v>2.057384203467334</v>
@@ -10000,7 +10000,7 @@
         <v>43.96639127163915</v>
       </c>
       <c r="I274">
-        <v>-8.622645099655852</v>
+        <v>-7.585914670254474</v>
       </c>
       <c r="J274">
         <v>-3.070759114333959</v>
@@ -10035,7 +10035,7 @@
         <v>29.89629512574029</v>
       </c>
       <c r="I275">
-        <v>-5.813130014172538</v>
+        <v>-4.084131929778531</v>
       </c>
       <c r="J275">
         <v>0.3252556885684192</v>
@@ -10070,7 +10070,7 @@
         <v>44.67927543405396</v>
       </c>
       <c r="I276">
-        <v>-5.192985948979585</v>
+        <v>-3.484989610007074</v>
       </c>
       <c r="J276">
         <v>-2.115366756214101</v>
@@ -10105,7 +10105,7 @@
         <v>29.38666115285305</v>
       </c>
       <c r="I277">
-        <v>-5.493696869657875</v>
+        <v>-3.757689418793991</v>
       </c>
       <c r="J277">
         <v>0.8280800521616749</v>
@@ -10140,7 +10140,7 @@
         <v>41.35139056614095</v>
       </c>
       <c r="I278">
-        <v>-5.571583063978484</v>
+        <v>-3.913136934500215</v>
       </c>
       <c r="J278">
         <v>-1.666377517497542</v>
@@ -10175,7 +10175,7 @@
         <v>44.18237105586013</v>
       </c>
       <c r="I279">
-        <v>-5.716544185832185</v>
+        <v>-4.262366401046073</v>
       </c>
       <c r="J279">
         <v>0.02919301245333567</v>
@@ -10210,7 +10210,7 @@
         <v>25.71666997247993</v>
       </c>
       <c r="I280">
-        <v>-5.431751803899926</v>
+        <v>-3.702431491465453</v>
       </c>
       <c r="J280">
         <v>-0.9989052022401264</v>
@@ -10245,7 +10245,7 @@
         <v>28.41428571428571</v>
       </c>
       <c r="I281">
-        <v>-4.294315791877028</v>
+        <v>-2.461087316734656</v>
       </c>
       <c r="J281">
         <v>0.4441911406010915</v>
@@ -10280,7 +10280,7 @@
         <v>22.86</v>
       </c>
       <c r="I282">
-        <v>-3.026519971161568</v>
+        <v>-1.234680534227574</v>
       </c>
       <c r="J282">
         <v>-0.2829162309382351</v>
@@ -10315,7 +10315,7 @@
         <v>26.43287671232877</v>
       </c>
       <c r="I283">
-        <v>-1.120982625194954</v>
+        <v>0.808750465631912</v>
       </c>
       <c r="J283">
         <v>1.079441381888112</v>
@@ -10350,7 +10350,7 @@
         <v>25.87826086956522</v>
       </c>
       <c r="I284">
-        <v>1.815447922893909</v>
+        <v>3.56976029713019</v>
       </c>
       <c r="J284">
         <v>-1.076143966248432</v>

</xml_diff>